<commit_message>
chore: update schedule.xlsx with latest changes
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matu\work\ToDo\vercal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF8A5BF-8D50-412A-AC1B-AE1F01042FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ED89AC-E604-4357-93F5-74F592AFD192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>period_start</t>
   </si>
@@ -108,6 +108,30 @@
   </si>
   <si>
     <t>AM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4月10日の予定</t>
+    <rPh sb="1" eb="2">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ニチ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヨテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2025-04-01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入学式</t>
+    <rPh sb="0" eb="3">
+      <t>ニュウガクシキ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -468,25 +492,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="12.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -532,7 +556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -552,7 +576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -575,7 +599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -596,6 +620,28 @@
       </c>
       <c r="G5" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>